<commit_message>
Comparator : work in progress
</commit_message>
<xml_diff>
--- a/OpenFisca/correspondances_variables.xlsx
+++ b/OpenFisca/correspondances_variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="14955" windowHeight="12855" activeTab="1"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="14955" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Malka Guillot:</t>
         </r>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Label absent dans OF : à rajouter</t>
@@ -7011,14 +7011,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -7319,6 +7319,11 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7337,11 +7342,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calcul" xfId="1" builtinId="22"/>
@@ -8822,7 +8822,7 @@
       <c r="L113" s="47"/>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="68" t="s">
+      <c r="A114" s="62" t="s">
         <v>2265</v>
       </c>
       <c r="B114" s="47" t="s">
@@ -10017,7 +10017,7 @@
       <c r="C208" s="48">
         <v>6</v>
       </c>
-      <c r="F208" s="70" t="s">
+      <c r="F208" s="64" t="s">
         <v>2271</v>
       </c>
       <c r="K208" s="47"/>
@@ -11919,7 +11919,7 @@
       <c r="A423" s="56" t="s">
         <v>1274</v>
       </c>
-      <c r="B423" s="69" t="s">
+      <c r="B423" s="63" t="s">
         <v>2132</v>
       </c>
       <c r="C423" s="58">
@@ -11927,10 +11927,10 @@
       </c>
       <c r="D423" s="58"/>
       <c r="E423" s="58"/>
-      <c r="F423" s="69" t="s">
+      <c r="F423" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="G423" s="69" t="s">
+      <c r="G423" s="63" t="s">
         <v>1677</v>
       </c>
     </row>
@@ -13133,8 +13133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA350"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15020,7 +15020,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="129" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
         <v>677</v>
       </c>
@@ -15028,7 +15028,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="130" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
         <v>679</v>
       </c>
@@ -15036,7 +15036,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="131" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
         <v>681</v>
       </c>
@@ -15044,7 +15044,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="132" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
         <v>682</v>
       </c>
@@ -15055,7 +15055,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="133" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
         <v>685</v>
       </c>
@@ -15066,7 +15066,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
         <v>688</v>
       </c>
@@ -15077,7 +15077,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="135" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
         <v>691</v>
       </c>
@@ -15088,7 +15088,10 @@
         <v>693</v>
       </c>
     </row>
-    <row r="136" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>1</v>
+      </c>
       <c r="C136" t="s">
         <v>694</v>
       </c>
@@ -15099,7 +15102,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="137" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
         <v>697</v>
       </c>
@@ -15110,7 +15113,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="138" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
         <v>700</v>
       </c>
@@ -15118,7 +15121,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="139" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
         <v>702</v>
       </c>
@@ -15126,7 +15129,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="140" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
         <v>704</v>
       </c>
@@ -15134,7 +15137,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="141" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
         <v>706</v>
       </c>
@@ -15151,7 +15154,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="142" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
         <v>711</v>
       </c>
@@ -15159,7 +15162,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="143" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
         <v>713</v>
       </c>
@@ -15170,7 +15173,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="144" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
         <v>715</v>
       </c>
@@ -15434,7 +15437,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="177" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C177" t="s">
         <v>781</v>
       </c>
@@ -15442,7 +15445,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="178" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C178" t="s">
         <v>782</v>
       </c>
@@ -15450,7 +15453,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="179" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
         <v>784</v>
       </c>
@@ -15458,7 +15461,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="180" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C180" t="s">
         <v>786</v>
       </c>
@@ -15466,7 +15469,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="181" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C181" t="s">
         <v>788</v>
       </c>
@@ -15474,7 +15477,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="182" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C182" t="s">
         <v>790</v>
       </c>
@@ -15482,7 +15485,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="183" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C183" t="s">
         <v>792</v>
       </c>
@@ -15490,7 +15493,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="184" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C184" t="s">
         <v>794</v>
       </c>
@@ -15498,7 +15501,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="185" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
         <v>796</v>
       </c>
@@ -15506,7 +15509,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="186" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C186" t="s">
         <v>798</v>
       </c>
@@ -15514,7 +15517,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="187" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C187" t="s">
         <v>800</v>
       </c>
@@ -15525,7 +15528,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="188" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C188" t="s">
         <v>803</v>
       </c>
@@ -15533,7 +15536,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="189" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C189" t="s">
         <v>805</v>
       </c>
@@ -15544,7 +15547,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="190" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C190" t="s">
         <v>808</v>
       </c>
@@ -15555,7 +15558,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="191" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C191" t="s">
         <v>811</v>
       </c>
@@ -15563,7 +15566,10 @@
         <v>812</v>
       </c>
     </row>
-    <row r="192" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>1</v>
+      </c>
       <c r="C192" t="s">
         <v>813</v>
       </c>
@@ -18928,7 +18934,7 @@
       <c r="J1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="65" t="s">
         <v>144</v>
       </c>
       <c r="M1" s="15" t="s">
@@ -18936,7 +18942,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="68" t="s">
         <v>156</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -18950,13 +18956,13 @@
         <v>14</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="L2" s="63"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="20" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
+      <c r="A3" s="68"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -18970,7 +18976,7 @@
       <c r="H3" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="L3" s="63"/>
+      <c r="L3" s="66"/>
       <c r="M3" s="16" t="s">
         <v>147</v>
       </c>
@@ -18984,7 +18990,7 @@
         <v>153</v>
       </c>
       <c r="J4" s="6"/>
-      <c r="L4" s="64"/>
+      <c r="L4" s="67"/>
       <c r="M4" s="17" t="s">
         <v>149</v>
       </c>
@@ -19387,7 +19393,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="69" t="s">
         <v>95</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -19397,7 +19403,7 @@
         <v>220</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="66" t="s">
+      <c r="H40" s="69" t="s">
         <v>213</v>
       </c>
       <c r="I40" s="10" t="s">
@@ -19405,7 +19411,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="66"/>
+      <c r="B41" s="69"/>
       <c r="C41" s="5" t="s">
         <v>215</v>
       </c>
@@ -19413,13 +19419,13 @@
         <v>221</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="66"/>
+      <c r="H41" s="69"/>
       <c r="I41" s="10" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="66"/>
+      <c r="B42" s="69"/>
       <c r="C42" s="5" t="s">
         <v>216</v>
       </c>
@@ -19427,7 +19433,7 @@
         <v>222</v>
       </c>
       <c r="G42" s="3"/>
-      <c r="H42" s="66"/>
+      <c r="H42" s="69"/>
       <c r="I42" s="10" t="s">
         <v>219</v>
       </c>
@@ -19444,7 +19450,7 @@
       <c r="E44" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="H44" s="67" t="s">
+      <c r="H44" s="70" t="s">
         <v>199</v>
       </c>
       <c r="I44" s="10" t="s">
@@ -19462,7 +19468,7 @@
       <c r="F45" s="11">
         <v>1</v>
       </c>
-      <c r="H45" s="67"/>
+      <c r="H45" s="70"/>
       <c r="I45" s="28" t="s">
         <v>196</v>
       </c>
@@ -19476,7 +19482,7 @@
       <c r="E46" t="s">
         <v>189</v>
       </c>
-      <c r="H46" s="66" t="s">
+      <c r="H46" s="69" t="s">
         <v>194</v>
       </c>
       <c r="I46" s="10" t="s">
@@ -19490,7 +19496,7 @@
       <c r="E47" t="s">
         <v>190</v>
       </c>
-      <c r="H47" s="66"/>
+      <c r="H47" s="69"/>
       <c r="I47" s="10" t="s">
         <v>193</v>
       </c>
@@ -19505,7 +19511,7 @@
       <c r="F48" s="11">
         <v>1</v>
       </c>
-      <c r="H48" s="66"/>
+      <c r="H48" s="69"/>
       <c r="I48" s="27" t="s">
         <v>181</v>
       </c>
@@ -19660,7 +19666,7 @@
       <c r="B61" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C61" s="69" t="s">
         <v>176</v>
       </c>
       <c r="D61" s="29"/>
@@ -19678,7 +19684,7 @@
       <c r="B62" t="s">
         <v>106</v>
       </c>
-      <c r="C62" s="66"/>
+      <c r="C62" s="69"/>
       <c r="D62" s="29"/>
       <c r="E62" s="25"/>
       <c r="F62" s="26"/>
@@ -19689,7 +19695,7 @@
         <v>169</v>
       </c>
       <c r="J62"/>
-      <c r="L62" s="66" t="s">
+      <c r="L62" s="69" t="s">
         <v>172</v>
       </c>
     </row>
@@ -19697,7 +19703,7 @@
       <c r="B63" t="s">
         <v>107</v>
       </c>
-      <c r="C63" s="66"/>
+      <c r="C63" s="69"/>
       <c r="D63" s="29"/>
       <c r="E63" s="25"/>
       <c r="F63" s="26"/>
@@ -19708,13 +19714,13 @@
         <v>170</v>
       </c>
       <c r="J63"/>
-      <c r="L63" s="66"/>
+      <c r="L63" s="69"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>108</v>
       </c>
-      <c r="C64" s="66"/>
+      <c r="C64" s="69"/>
       <c r="D64" s="29"/>
       <c r="E64" s="25"/>
       <c r="F64" s="26"/>
@@ -19725,7 +19731,7 @@
         <v>171</v>
       </c>
       <c r="J64"/>
-      <c r="L64" s="66"/>
+      <c r="L64" s="69"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" t="s">

</xml_diff>

<commit_message>
variables to calculate pfam
</commit_message>
<xml_diff>
--- a/OpenFisca/correspondances_variables.xlsx
+++ b/OpenFisca/correspondances_variables.xlsx
@@ -15443,8 +15443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187:D187"/>
+    <sheetView tabSelected="1" topLeftCell="A314" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C332" sqref="C332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19221,7 +19221,7 @@
         <v>1</v>
       </c>
       <c r="C332" t="s">
-        <v>1083</v>
+        <v>1128</v>
       </c>
       <c r="D332" t="s">
         <v>1083</v>

</xml_diff>

<commit_message>
Update + waterfall revisite
Possibility to begin by salbrut
</commit_message>
<xml_diff>
--- a/OpenFisca/correspondances_variables.xlsx
+++ b/OpenFisca/correspondances_variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="645" windowWidth="14430" windowHeight="12195" activeTab="1"/>
+    <workbookView xWindow="14385" yWindow="705" windowWidth="14430" windowHeight="12135" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="7" r:id="rId1"/>
@@ -15446,8 +15446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B182" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView topLeftCell="B311" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G351" sqref="G351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19213,7 +19213,7 @@
         <v>1</v>
       </c>
       <c r="C331" t="s">
-        <v>1084</v>
+        <v>1129</v>
       </c>
       <c r="D331" t="s">
         <v>1084</v>
@@ -26413,8 +26413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA116"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:B66"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add variables on capital
</commit_message>
<xml_diff>
--- a/OpenFisca/correspondances_variables.xlsx
+++ b/OpenFisca/correspondances_variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="705" windowWidth="14430" windowHeight="12135" activeTab="8"/>
+    <workbookView xWindow="14385" yWindow="765" windowWidth="14430" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="7" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="3015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3828" uniqueCount="3015">
   <si>
     <t>id_indiv</t>
   </si>
@@ -10002,10 +10002,10 @@
   <dimension ref="A1:L523"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B442" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B399" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A462" sqref="A462"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15446,8 +15446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA362"/>
   <sheetViews>
-    <sheetView topLeftCell="B311" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G351" sqref="G351"/>
+    <sheetView tabSelected="1" topLeftCell="B98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17249,16 +17249,28 @@
       </c>
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
+      <c r="B112" s="19">
+        <v>1</v>
+      </c>
+      <c r="C112" s="19" t="s">
         <v>640</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>377</v>
       </c>
       <c r="N112" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="113" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
+      <c r="B113" s="19">
+        <v>1</v>
+      </c>
+      <c r="C113" s="19" t="s">
         <v>642</v>
+      </c>
+      <c r="D113" s="19" t="s">
+        <v>388</v>
       </c>
       <c r="N113" t="s">
         <v>643</v>
@@ -17387,16 +17399,28 @@
       </c>
     </row>
     <row r="127" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C127" t="s">
+      <c r="B127" s="19">
+        <v>1</v>
+      </c>
+      <c r="C127" s="19" t="s">
         <v>671</v>
+      </c>
+      <c r="D127" s="19" t="s">
+        <v>264</v>
       </c>
       <c r="N127" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="128" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
+      <c r="B128" s="19">
+        <v>1</v>
+      </c>
+      <c r="C128" s="19" t="s">
         <v>672</v>
+      </c>
+      <c r="D128" s="19" t="s">
+        <v>271</v>
       </c>
       <c r="N128" t="s">
         <v>673</v>
@@ -18609,7 +18633,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="257" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C257" t="s">
         <v>958</v>
       </c>
@@ -18617,7 +18641,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="258" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C258" t="s">
         <v>960</v>
       </c>
@@ -18625,23 +18649,35 @@
         <v>961</v>
       </c>
     </row>
-    <row r="259" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C259" t="s">
+    <row r="259" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B259" s="19">
+        <v>1</v>
+      </c>
+      <c r="C259" s="19" t="s">
         <v>962</v>
+      </c>
+      <c r="D259" s="19" t="s">
+        <v>354</v>
       </c>
       <c r="N259" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="260" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C260" t="s">
+    <row r="260" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B260" s="19">
+        <v>1</v>
+      </c>
+      <c r="C260" s="19" t="s">
         <v>964</v>
+      </c>
+      <c r="D260" s="19" t="s">
+        <v>369</v>
       </c>
       <c r="N260" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="261" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C261" t="s">
         <v>966</v>
       </c>
@@ -18649,7 +18685,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="262" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C262" t="s">
         <v>968</v>
       </c>
@@ -18657,7 +18693,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="263" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C263" t="s">
         <v>969</v>
       </c>
@@ -18665,7 +18701,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="264" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C264" t="s">
         <v>971</v>
       </c>
@@ -18673,7 +18709,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="265" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C265" t="s">
         <v>973</v>
       </c>
@@ -18681,7 +18717,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="266" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C266" t="s">
         <v>975</v>
       </c>
@@ -18689,7 +18725,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="267" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C267" t="s">
         <v>977</v>
       </c>
@@ -18697,7 +18733,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="268" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C268" t="s">
         <v>979</v>
       </c>
@@ -18705,7 +18741,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="269" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C269" t="s">
         <v>981</v>
       </c>
@@ -18713,7 +18749,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="270" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C270" t="s">
         <v>983</v>
       </c>
@@ -18721,7 +18757,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="271" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C271" t="s">
         <v>985</v>
       </c>
@@ -18729,7 +18765,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="272" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C272" t="s">
         <v>987</v>
       </c>
@@ -26413,7 +26449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>

</xml_diff>